<commit_message>
Corrección de los resultados de Nevasa obtenidos el 20231008.
</commit_message>
<xml_diff>
--- a/Nevasa/InformeCompleto/20241008/20241008_informe_completo_results.xlsx
+++ b/Nevasa/InformeCompleto/20241008/20241008_informe_completo_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,19 +496,19 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>45573</v>
+        <v>45574</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>45572</v>
+        <v>45573</v>
       </c>
       <c r="D2" t="n">
-        <v>0.48</v>
+        <v>0.49</v>
       </c>
       <c r="E2" t="n">
-        <v>588094080</v>
+        <v>147024010</v>
       </c>
       <c r="F2" t="n">
-        <v>588000000</v>
+        <v>147000000</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -526,6 +526,366 @@
       <c r="J2" t="inlineStr">
         <is>
           <t>PACTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>FONDO DE INVERSION NEVASA AHORRO</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>45573</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>45573</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F3" t="n">
+        <v>76027595</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>BCHIEJ0717</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>VENTA</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>RENTA FIJA</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>FONDO DE INVERSION NEVASA AHORRO</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>45573</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>45573</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2.51</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F4" t="n">
+        <v>80139302</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>BESTJ41008</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>VENTA</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>RENTA FIJA</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>FONDO DE INVERSION NEVASA AHORRO</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>45573</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>45573</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2.21</v>
+      </c>
+      <c r="E5" t="n">
+        <v>15500</v>
+      </c>
+      <c r="F5" t="n">
+        <v>597519830</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>BBBVK61113</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>VENTA</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>RENTA FIJA</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>FONDO DE INVERSION NEVASA AHORRO</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>45573</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>45573</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2.51</v>
+      </c>
+      <c r="E6" t="n">
+        <v>5000</v>
+      </c>
+      <c r="F6" t="n">
+        <v>200348256</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>BESTJ41008</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>VENTA</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>RENTA FIJA</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>FONDO DE INVERSION NEVASA AHORRO</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>45573</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>45573</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>33025154.912</v>
+      </c>
+      <c r="F7" t="n">
+        <v>33012410</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>SOCOVESA</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>VENTA</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>SIMULTANEA</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>FONDO DE INVERSION NEVASA AHORRO</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>45573</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>45573</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>390210469.11</v>
+      </c>
+      <c r="F8" t="n">
+        <v>390000887</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>BESALCO</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>VENTA</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>SIMULTANEA</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>FONDO DE INVERSION NEVASA AHORRO</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>45573</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>45573</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>30621570</v>
+      </c>
+      <c r="F9" t="n">
+        <v>30471350</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>LTM</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>VENTA</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>SIMULTANEA</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>FONDO DE INVERSION NEVASA AHORRO</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>45573</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>45573</v>
+      </c>
+      <c r="D10" t="n">
+        <v>16532.39</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2773</v>
+      </c>
+      <c r="F10" t="n">
+        <v>45844317</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>CFINHRFLA</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>VENTA</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>RENTA VARIABLE</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>FONDO DE INVERSION NEVASA AHORRO</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>45573</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>45573</v>
+      </c>
+      <c r="D11" t="n">
+        <v>15976.83</v>
+      </c>
+      <c r="E11" t="n">
+        <v>557</v>
+      </c>
+      <c r="F11" t="n">
+        <v>8899095</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>CFINHRFLB</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>COMPRA</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>RENTA VARIABLE</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Se modifica el campo fecha_pago de las rentas fijas en el informe Nevasa
Ahora utiliza el siguiente día hábil como fecha de pago, de momento solo considera fines de semana como no hábiles, quedaría agregar los días festivos.
</commit_message>
<xml_diff>
--- a/Nevasa/InformeCompleto/20241008/20241008_informe_completo_results.xlsx
+++ b/Nevasa/InformeCompleto/20241008/20241008_informe_completo_results.xlsx
@@ -536,7 +536,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45573</v>
+        <v>45574</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>45573</v>
@@ -576,7 +576,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>45573</v>
+        <v>45574</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>45573</v>
@@ -616,7 +616,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>45573</v>
+        <v>45574</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>45573</v>
@@ -656,7 +656,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>45573</v>
+        <v>45574</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>45573</v>

</xml_diff>